<commit_message>
feat: commited all data related changes (inputs, outputs, solutions, etc)
</commit_message>
<xml_diff>
--- a/data/inputs/viajes_prueba/test_VBCN2501598.xlsx
+++ b/data/inputs/viajes_prueba/test_VBCN2501598.xlsx
@@ -574,7 +574,7 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -647,7 +647,7 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
@@ -720,7 +720,7 @@
         </is>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
@@ -793,7 +793,7 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
@@ -866,7 +866,7 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
@@ -939,7 +939,7 @@
         </is>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
@@ -1085,7 +1085,7 @@
         </is>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
@@ -1158,7 +1158,7 @@
         </is>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
@@ -1231,7 +1231,7 @@
         </is>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>
@@ -1304,7 +1304,7 @@
         </is>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
@@ -1377,7 +1377,7 @@
         </is>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13" t="inlineStr">
         <is>
@@ -1450,7 +1450,7 @@
         </is>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14" t="inlineStr">
         <is>
@@ -1523,7 +1523,7 @@
         </is>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" t="inlineStr">
         <is>
@@ -1596,7 +1596,7 @@
         </is>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" t="inlineStr">
         <is>
@@ -1669,7 +1669,7 @@
         </is>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" t="inlineStr">
         <is>
@@ -1742,7 +1742,7 @@
         </is>
       </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18" t="inlineStr">
         <is>
@@ -1815,7 +1815,7 @@
         </is>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19" t="inlineStr">
         <is>
@@ -1888,7 +1888,7 @@
         </is>
       </c>
       <c r="K20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20" t="inlineStr">
         <is>
@@ -1961,7 +1961,7 @@
         </is>
       </c>
       <c r="K21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21" t="inlineStr">
         <is>
@@ -2034,7 +2034,7 @@
         </is>
       </c>
       <c r="K22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" t="inlineStr">
         <is>
@@ -2107,7 +2107,7 @@
         </is>
       </c>
       <c r="K23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23" t="inlineStr">
         <is>
@@ -2180,7 +2180,7 @@
         </is>
       </c>
       <c r="K24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
         </is>
       </c>
       <c r="K25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25" t="inlineStr">
         <is>
@@ -2326,7 +2326,7 @@
         </is>
       </c>
       <c r="K26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L26" t="inlineStr">
         <is>
@@ -2397,7 +2397,7 @@
         </is>
       </c>
       <c r="K27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L27" t="inlineStr">
         <is>
@@ -2470,7 +2470,7 @@
         </is>
       </c>
       <c r="K28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L28" t="inlineStr">
         <is>
@@ -2541,7 +2541,7 @@
         </is>
       </c>
       <c r="K29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L29" t="inlineStr">
         <is>
@@ -2612,7 +2612,7 @@
         </is>
       </c>
       <c r="K30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L30" t="inlineStr">
         <is>
@@ -2685,7 +2685,7 @@
         </is>
       </c>
       <c r="K31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L31" t="inlineStr">
         <is>
@@ -2758,7 +2758,7 @@
         </is>
       </c>
       <c r="K32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L32" t="inlineStr">
         <is>
@@ -2831,7 +2831,7 @@
         </is>
       </c>
       <c r="K33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L33" t="inlineStr">
         <is>
@@ -2904,7 +2904,7 @@
         </is>
       </c>
       <c r="K34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L34" t="inlineStr">
         <is>
@@ -3415,7 +3415,7 @@
         </is>
       </c>
       <c r="K41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L41" t="inlineStr">
         <is>
@@ -3707,7 +3707,7 @@
         </is>
       </c>
       <c r="K45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L45" t="inlineStr">
         <is>
@@ -3780,7 +3780,7 @@
         </is>
       </c>
       <c r="K46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L46" t="inlineStr">
         <is>
@@ -3853,7 +3853,7 @@
         </is>
       </c>
       <c r="K47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L47" t="inlineStr">
         <is>
@@ -4072,7 +4072,7 @@
         </is>
       </c>
       <c r="K50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L50" t="inlineStr">
         <is>
@@ -4145,7 +4145,7 @@
         </is>
       </c>
       <c r="K51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L51" t="inlineStr">
         <is>
@@ -4218,7 +4218,7 @@
         </is>
       </c>
       <c r="K52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L52" t="inlineStr">
         <is>
@@ -4291,7 +4291,7 @@
         </is>
       </c>
       <c r="K53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L53" t="inlineStr">
         <is>
@@ -4364,7 +4364,7 @@
         </is>
       </c>
       <c r="K54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L54" t="inlineStr">
         <is>
@@ -4437,7 +4437,7 @@
         </is>
       </c>
       <c r="K55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L55" t="inlineStr">
         <is>
@@ -4510,7 +4510,7 @@
         </is>
       </c>
       <c r="K56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L56" t="inlineStr">
         <is>

</xml_diff>